<commit_message>
New Test Data File
</commit_message>
<xml_diff>
--- a/CIDBankCDCalculator/Data/Test data.xlsx
+++ b/CIDBankCDCalculator/Data/Test data.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Initial Deposit Amount</t>
   </si>
@@ -51,13 +46,22 @@
   </si>
   <si>
     <t>Anually</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Correct CD</t>
+  </si>
+  <si>
+    <t>Expected CD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +74,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,10 +115,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -115,9 +127,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -210,7 +227,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -387,7 +404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,173 +412,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>3200</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
+      <c r="D4" s="4">
+        <v>0.01</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>365</v>
+      </c>
+      <c r="G4">
+        <f>B4*(1+D4/F4)^(F4*C4/12)</f>
+        <v>3208.0098984772071</v>
+      </c>
+      <c r="H4">
+        <v>3208.0098984772071</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>6050</v>
       </c>
       <c r="C5" s="2">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
-        <v>12</v>
+      <c r="D5" s="4">
+        <v>0.12</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:H13" si="0">B5*(1+D5/F5)^(F5*C5/12)</f>
+        <v>6749.7934973251649</v>
+      </c>
+      <c r="H5">
+        <v>6749.7934973251649</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>14900</v>
       </c>
       <c r="C6" s="2">
         <v>14</v>
       </c>
-      <c r="D6" s="2">
-        <v>23</v>
+      <c r="D6" s="4">
+        <v>0.23</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>19341.702097494024</v>
+      </c>
+      <c r="H6">
+        <v>19341.702097494024</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>15500</v>
       </c>
       <c r="C7" s="2">
         <v>21</v>
       </c>
-      <c r="D7" s="2">
-        <v>34</v>
+      <c r="D7" s="4">
+        <v>0.34</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>26852.34474651613</v>
+      </c>
+      <c r="H7">
+        <v>26852.34474651613</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>20400</v>
       </c>
       <c r="C8" s="2">
         <v>28</v>
       </c>
-      <c r="D8" s="2">
-        <v>45</v>
+      <c r="D8" s="4">
+        <v>0.45</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>48546.229646046922</v>
+      </c>
+      <c r="H8">
+        <v>48546.229646046922</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>29000</v>
       </c>
       <c r="C9" s="2">
         <v>35</v>
       </c>
-      <c r="D9" s="2">
-        <v>56</v>
+      <c r="D9" s="4">
+        <v>0.56000000000000005</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>365</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>148320.79700967509</v>
+      </c>
+      <c r="H9">
+        <v>78578.059299999994</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>31000</v>
       </c>
       <c r="C10" s="2">
         <v>42</v>
       </c>
-      <c r="D10" s="2">
-        <v>67</v>
+      <c r="D10" s="4">
+        <v>0.67</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>303645.73466859577</v>
+      </c>
+      <c r="H10">
+        <v>498576.06900000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>38000</v>
       </c>
       <c r="C11" s="2">
         <v>43</v>
       </c>
-      <c r="D11" s="2">
-        <v>78</v>
+      <c r="D11" s="4">
+        <v>0.78</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>488341.43197247345</v>
+      </c>
+      <c r="H11">
+        <v>502379.02947000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>44700</v>
       </c>
       <c r="C12" s="2">
         <v>50</v>
       </c>
-      <c r="D12" s="2">
-        <v>89</v>
+      <c r="D12" s="4">
+        <v>0.89</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>960593.36428658641</v>
+      </c>
+      <c r="H12">
+        <v>945981.4632</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>49300</v>
       </c>
       <c r="C13" s="2">
         <v>57</v>
       </c>
-      <c r="D13" s="2">
-        <v>100</v>
+      <c r="D13" s="4">
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1326598.18470426</v>
+      </c>
+      <c r="H13">
+        <v>1236474.1839999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>